<commit_message>
Adicao de 2 telas, alem do save apos fechar. Transformado em app para desktop
</commit_message>
<xml_diff>
--- a/folha_pagamento.xlsx
+++ b/folha_pagamento.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +484,142 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Livia</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>atendente</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>480</v>
+      </c>
+      <c r="I2" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Grace</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>atendente</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>360</v>
+      </c>
+      <c r="I3" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lucas</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>subgerente</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H4" t="n">
+        <v>800</v>
+      </c>
+      <c r="I4" t="n">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cleria</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>gerente</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ficou apos expediente</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>886</v>
+      </c>
+      <c r="I5" t="n">
+        <v>886</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>